<commit_message>
adding genes to gviz and making document of progress
</commit_message>
<xml_diff>
--- a/results/all_cluster_mapping.xlsx
+++ b/results/all_cluster_mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">cluster</t>
   </si>
@@ -68,18 +68,24 @@
     <t xml:space="preserve">transitional_to_acinar1</t>
   </si>
   <si>
+    <t xml:space="preserve">Endo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
     <t xml:space="preserve">undetermined</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
@@ -125,6 +131,9 @@
     <t xml:space="preserve">centroacinar</t>
   </si>
   <si>
+    <t xml:space="preserve">Endo3</t>
+  </si>
+  <si>
     <t xml:space="preserve">endothelial_cell</t>
   </si>
   <si>
@@ -146,7 +155,7 @@
     <t xml:space="preserve">13</t>
   </si>
   <si>
-    <t xml:space="preserve">Endo1</t>
+    <t xml:space="preserve">EP2</t>
   </si>
   <si>
     <t xml:space="preserve">Prolif_acinar</t>
@@ -600,7 +609,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -608,10 +617,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -637,10 +646,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -652,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
@@ -661,12 +670,12 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -695,10 +704,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -724,7 +733,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -739,7 +748,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
@@ -748,15 +757,15 @@
         <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -774,7 +783,7 @@
         <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
@@ -782,11 +791,11 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -797,13 +806,13 @@
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
@@ -811,7 +820,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -832,7 +841,7 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
@@ -840,7 +849,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -915,7 +924,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -927,7 +936,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -936,7 +945,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -950,7 +959,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -962,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -973,13 +982,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -991,7 +1000,7 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -999,10 +1008,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1020,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -1028,10 +1037,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1043,7 +1052,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -1052,15 +1061,15 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1072,7 +1081,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -1086,10 +1095,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1101,7 +1110,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -1115,10 +1124,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1130,7 +1139,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1139,15 +1148,15 @@
         <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1159,7 +1168,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
@@ -1168,15 +1177,15 @@
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1188,7 +1197,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -1197,15 +1206,15 @@
         <v>15</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1217,7 +1226,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -1226,21 +1235,21 @@
         <v>15</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1252,7 +1261,7 @@
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
@@ -1306,28 +1315,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -1335,7 +1344,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1347,7 +1356,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -1364,7 +1373,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1376,24 +1385,24 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1405,13 +1414,13 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -1419,10 +1428,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1434,7 +1443,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -1448,10 +1457,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1463,7 +1472,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -1472,44 +1481,44 @@
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1521,7 +1530,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -1530,44 +1539,44 @@
         <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1579,7 +1588,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -1588,15 +1597,15 @@
         <v>15</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1608,13 +1617,13 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
@@ -1622,10 +1631,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1637,13 +1646,13 @@
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -1697,7 +1706,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1709,16 +1718,16 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -1726,7 +1735,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1738,53 +1747,53 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1796,24 +1805,24 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1825,7 +1834,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -1839,10 +1848,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1854,24 +1863,24 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1883,13 +1892,13 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -1897,60 +1906,60 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2001,7 +2010,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -2013,16 +2022,16 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -2030,7 +2039,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -2042,16 +2051,16 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -2059,36 +2068,36 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -2106,7 +2115,7 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
@@ -2114,10 +2123,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2129,30 +2138,30 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -2164,7 +2173,7 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
         <v>14</v>
@@ -2172,10 +2181,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -2187,13 +2196,13 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -2201,10 +2210,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -2216,13 +2225,13 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
@@ -2230,10 +2239,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -2245,24 +2254,24 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -2274,24 +2283,24 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -2303,45 +2312,45 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2392,7 +2401,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -2404,16 +2413,16 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -2421,7 +2430,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -2433,42 +2442,42 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -2476,10 +2485,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -2491,42 +2500,42 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
@@ -2534,28 +2543,28 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -2563,10 +2572,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -2578,13 +2587,13 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -2592,28 +2601,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
@@ -2621,31 +2630,31 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2714,7 +2723,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -2743,7 +2752,7 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -2754,7 +2763,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -2772,7 +2781,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
         <v>13</v>
@@ -2780,10 +2789,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -2801,7 +2810,7 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -2809,10 +2818,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2824,21 +2833,21 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -2859,7 +2868,7 @@
         <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -2867,10 +2876,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -2888,7 +2897,7 @@
         <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>14</v>
@@ -2896,10 +2905,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -2917,7 +2926,7 @@
         <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
@@ -2925,7 +2934,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -2946,7 +2955,7 @@
         <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
@@ -2954,10 +2963,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -2975,7 +2984,7 @@
         <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -2983,10 +2992,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -2998,24 +3007,24 @@
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -3033,7 +3042,7 @@
         <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -3041,7 +3050,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3062,7 +3071,7 @@
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
@@ -3070,31 +3079,31 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3145,25 +3154,25 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -3174,7 +3183,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -3186,13 +3195,13 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -3203,7 +3212,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -3215,7 +3224,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -3224,12 +3233,12 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3244,24 +3253,24 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -3273,7 +3282,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -3282,15 +3291,15 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -3302,7 +3311,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -3311,15 +3320,15 @@
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -3331,7 +3340,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -3340,15 +3349,15 @@
         <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -3360,7 +3369,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -3369,15 +3378,15 @@
         <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -3389,13 +3398,13 @@
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
@@ -3403,28 +3412,28 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -3432,10 +3441,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -3453,7 +3462,7 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
@@ -3461,7 +3470,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3470,19 +3479,19 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
@@ -3490,31 +3499,31 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
       <c r="G14" t="s">
         <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3571,19 +3580,19 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -3594,7 +3603,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -3606,7 +3615,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -3615,7 +3624,7 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -3623,7 +3632,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -3635,7 +3644,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -3649,22 +3658,22 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -3678,7 +3687,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3687,19 +3696,19 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -3707,10 +3716,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -3722,24 +3731,24 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -3751,7 +3760,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -3760,15 +3769,15 @@
         <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -3780,7 +3789,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -3794,10 +3803,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -3809,7 +3818,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -3818,12 +3827,12 @@
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3832,13 +3841,13 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -3852,10 +3861,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -3867,7 +3876,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -3881,10 +3890,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -3896,7 +3905,7 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -3905,12 +3914,12 @@
         <v>15</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3919,19 +3928,19 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
@@ -3939,10 +3948,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -3954,7 +3963,7 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -3963,15 +3972,15 @@
         <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -3983,13 +3992,13 @@
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
@@ -4043,7 +4052,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -4055,13 +4064,13 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -4072,7 +4081,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -4084,13 +4093,13 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -4119,7 +4128,7 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -4127,10 +4136,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -4142,13 +4151,13 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -4156,10 +4165,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -4171,24 +4180,24 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -4200,13 +4209,13 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -4214,10 +4223,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -4235,7 +4244,7 @@
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -4243,16 +4252,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -4264,7 +4273,7 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
@@ -4272,10 +4281,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -4287,13 +4296,13 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
@@ -4301,10 +4310,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -4316,13 +4325,13 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -4330,10 +4339,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -4345,13 +4354,13 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
@@ -4359,10 +4368,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -4374,24 +4383,24 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -4403,30 +4412,30 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -4438,7 +4447,7 @@
         <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
@@ -4446,10 +4455,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -4461,13 +4470,13 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>

</xml_diff>